<commit_message>
Minor changes to meeting details
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rinbaruah/Monash Business School Local/Master of Business Analytics  /Exploratory Data Analysis/Assignments/Assignment 3/assignment-3-seekers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD1A0CF-8AA0-ED49-9CB2-DEB9B2E01DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B62563F-6073-EC4A-9F36-D898C4A0E587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7120" yWindow="820" windowWidth="27860" windowHeight="16940" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>Assignment repository clone, assignment brief analysed and next meeting date scheduled.</t>
   </si>
   <si>
-    <t>Wild thing finalised as "Barking Owls". Data pulled using the Galah API. Next steps discussed briefly.</t>
-  </si>
-  <si>
     <t>Discussion on the approach for the analysis to be done.</t>
+  </si>
+  <si>
+    <t>Wild thing finalised as "Taipan". Data pulled using the Galah API. Next steps discussed briefly.</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +546,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated diary meeting and AI scripts
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aishwarya Kumar\Monash\sem2\ETC5521\assessment\assignment3\assignment-3-seekers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B530AF77-392A-43C0-A074-304A78860CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714A0907-FB15-418C-8266-2301C6A21684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Team Name:</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Report formatting style discussed and implemented.</t>
+  </si>
+  <si>
+    <t>Discussion on the approach for weather station integration. Next meeting date scheduled.</t>
+  </si>
+  <si>
+    <t>summary and conclusion discussed and implemeneted</t>
+  </si>
+  <si>
+    <t>Report formatting done and finalised</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -606,6 +615,57 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A12" s="2">
+        <v>45197</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A13" s="2">
+        <v>45201</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A14" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.875</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
third group meeting update
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aishwarya Kumar\Monash\sem2\ETC5521\assessment\assignment3\assignment-3-seekers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Desktop/ETC5521 - Exploratory data analysis/Assignment/assignment-3-seekers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714A0907-FB15-418C-8266-2301C6A21684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D44427-C8CA-CF43-939D-F8495F412527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="15080" yWindow="500" windowWidth="21620" windowHeight="17020" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Team Name:</t>
   </si>
@@ -94,6 +94,27 @@
   </si>
   <si>
     <t>Report formatting done and finalised</t>
+  </si>
+  <si>
+    <t>Part 2 Group Members:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completing handover process from part 1 group member Arindom. </t>
+  </si>
+  <si>
+    <t>Minghao Zeng</t>
+  </si>
+  <si>
+    <t>Discussion on how to approach the assignment. All members agreed to complete the whole assignment by 22/10/2023 and compare/merge the results afterward.</t>
+  </si>
+  <si>
+    <t>Tashya Sathyajit</t>
+  </si>
+  <si>
+    <t>Disha Rathod</t>
+  </si>
+  <si>
+    <t>New files from template repo added to assignment repo</t>
   </si>
 </sst>
 </file>
@@ -471,22 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.6875" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.3125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -505,15 +526,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -530,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45182</v>
       </c>
@@ -547,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45186</v>
       </c>
@@ -564,7 +585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45187</v>
       </c>
@@ -581,7 +602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45194</v>
       </c>
@@ -598,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45195</v>
       </c>
@@ -615,7 +636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45197</v>
       </c>
@@ -632,7 +653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45201</v>
       </c>
@@ -649,7 +670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45204</v>
       </c>
@@ -664,6 +685,93 @@
       </c>
       <c r="E14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>45211</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>45214</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>45214</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update on meeting summary
</commit_message>
<xml_diff>
--- a/assign03_meeting_diary.xlsx
+++ b/assign03_meeting_diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Desktop/ETC5521 - Exploratory data analysis/Assignment/assignment-3-seekers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D44427-C8CA-CF43-939D-F8495F412527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F3CF3B-0674-2140-A4E2-5E77F2DD13FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="500" windowWidth="21620" windowHeight="17020" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
+    <workbookView xWindow="13160" yWindow="500" windowWidth="21620" windowHeight="21100" xr2:uid="{AA36F377-8185-6045-958F-09DEEBD07722}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Team Name:</t>
   </si>
@@ -115,6 +115,21 @@
   </si>
   <si>
     <t>New files from template repo added to assignment repo</t>
+  </si>
+  <si>
+    <t>Agreed to complete task 1 by 20/10/2023 and meet up again for the findings</t>
+  </si>
+  <si>
+    <t>Discuss findings of task 1 and set deadline for task 2 on 23/10/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discuss findings of task 2 and discuss on how to write up introduction and data description </t>
+  </si>
+  <si>
+    <t>Discuss on minor errors on visual inference and finalise the summary part</t>
+  </si>
+  <si>
+    <t>Finalise the entire report and film the presentation with the other group</t>
   </si>
 </sst>
 </file>
@@ -492,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B0CB73-A0EE-1845-ADEE-622320F90FF1}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,6 +789,91 @@
         <v>26</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>45215</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>45219</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>45222</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>45224</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>